<commit_message>
areas 1 to 4 in dictionary
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="195">
   <si>
     <t>English Communication / Area 1</t>
   </si>
@@ -28,7 +28,16 @@
     <t>Social and Behavioral Sciences / Area 4</t>
   </si>
   <si>
-    <t>Physical and Biological Sciences / Area 5</t>
+    <t>Lab Area 5A</t>
+  </si>
+  <si>
+    <t>Non Lab 5A</t>
+  </si>
+  <si>
+    <t>Lab 5B</t>
+  </si>
+  <si>
+    <t>Non Lab 5B</t>
   </si>
   <si>
     <t>ENGL 101A</t>
@@ -43,6 +52,21 @@
     <t>ASL 103A</t>
   </si>
   <si>
+    <t>AJ 108</t>
+  </si>
+  <si>
+    <t>ASTR 101A &amp; 102</t>
+  </si>
+  <si>
+    <t>ASTR 101A</t>
+  </si>
+  <si>
+    <t>ANTH 101</t>
+  </si>
+  <si>
+    <t>BIOL 105</t>
+  </si>
+  <si>
     <t>ENGL 101C</t>
   </si>
   <si>
@@ -55,6 +79,18 @@
     <t>ASL 104A</t>
   </si>
   <si>
+    <t>ASTR 101B &amp; 102</t>
+  </si>
+  <si>
+    <t>ASTR 101B</t>
+  </si>
+  <si>
+    <t>BIOL 101A</t>
+  </si>
+  <si>
+    <t>BIOL 107</t>
+  </si>
+  <si>
     <t>COMM 111</t>
   </si>
   <si>
@@ -67,6 +103,21 @@
     <t>CHIN 102A</t>
   </si>
   <si>
+    <t>ANTH 102</t>
+  </si>
+  <si>
+    <t>CHEM 101A</t>
+  </si>
+  <si>
+    <t>CHEM 108</t>
+  </si>
+  <si>
+    <t>BIOL 101B</t>
+  </si>
+  <si>
+    <t>BIOL 109</t>
+  </si>
+  <si>
     <t>MATH 103</t>
   </si>
   <si>
@@ -76,6 +127,21 @@
     <t>CHIN 102B</t>
   </si>
   <si>
+    <t>ANTH 103</t>
+  </si>
+  <si>
+    <t>CHEM 101B</t>
+  </si>
+  <si>
+    <t>ENVS 110</t>
+  </si>
+  <si>
+    <t>BIOL 103A</t>
+  </si>
+  <si>
+    <t>BIOL 141</t>
+  </si>
+  <si>
     <t>MATH 104</t>
   </si>
   <si>
@@ -85,6 +151,21 @@
     <t>CHS 102A</t>
   </si>
   <si>
+    <t>ANTH 104</t>
+  </si>
+  <si>
+    <t>CHEM 102</t>
+  </si>
+  <si>
+    <t>GEOL 102</t>
+  </si>
+  <si>
+    <t>BIOL 103B</t>
+  </si>
+  <si>
+    <t>ENVS 108</t>
+  </si>
+  <si>
     <t>MATH 156</t>
   </si>
   <si>
@@ -94,6 +175,18 @@
     <t>CHS 102B</t>
   </si>
   <si>
+    <t>ANTH 106</t>
+  </si>
+  <si>
+    <t>CHEM 109</t>
+  </si>
+  <si>
+    <t>GEOL 103</t>
+  </si>
+  <si>
+    <t>BIOL 104</t>
+  </si>
+  <si>
     <t>MATH 159</t>
   </si>
   <si>
@@ -103,6 +196,18 @@
     <t>CHS 106A</t>
   </si>
   <si>
+    <t>ANTH 107</t>
+  </si>
+  <si>
+    <t>CHEM 112A</t>
+  </si>
+  <si>
+    <t>GEOL 104</t>
+  </si>
+  <si>
+    <t>BIOL 106</t>
+  </si>
+  <si>
     <t>MATH 188</t>
   </si>
   <si>
@@ -112,120 +217,228 @@
     <t>CHS 112</t>
   </si>
   <si>
+    <t>ANTH 108</t>
+  </si>
+  <si>
+    <t>CHEM 112B</t>
+  </si>
+  <si>
+    <t>PHYS 108</t>
+  </si>
+  <si>
+    <t>BIOL 130</t>
+  </si>
+  <si>
     <t>HIST 143</t>
   </si>
   <si>
     <t>ENGL 101B</t>
   </si>
   <si>
+    <t>BA 102A</t>
+  </si>
+  <si>
+    <t>GEOG 101</t>
+  </si>
+  <si>
+    <t>BIOL 142</t>
+  </si>
+  <si>
     <t xml:space="preserve">IS 100 </t>
   </si>
   <si>
     <t>ENGL 104</t>
   </si>
   <si>
+    <t>BA 102B</t>
+  </si>
+  <si>
+    <t>GEOL 101</t>
+  </si>
+  <si>
+    <t>ENVS 142</t>
+  </si>
+  <si>
     <t>IS 142</t>
   </si>
   <si>
     <t>ENGL 106</t>
   </si>
   <si>
+    <t>BA 142</t>
+  </si>
+  <si>
+    <t>GEOL 102 &amp; 102L</t>
+  </si>
+  <si>
     <t>IS 143</t>
   </si>
   <si>
     <t>ENGL 107</t>
   </si>
   <si>
+    <t>BRDC 155</t>
+  </si>
+  <si>
+    <t>GEOL 103 &amp; 103L</t>
+  </si>
+  <si>
     <t>MUS 100</t>
   </si>
   <si>
     <t>ENGL 109</t>
   </si>
   <si>
+    <t>CHS 101</t>
+  </si>
+  <si>
+    <t>GEOL 104 &amp; 104L</t>
+  </si>
+  <si>
     <t>MUS 101</t>
   </si>
   <si>
     <t>ENGL 112</t>
   </si>
   <si>
+    <t>PHYS 120</t>
+  </si>
+  <si>
     <t>MUS 102</t>
   </si>
   <si>
     <t>ENGL 113</t>
   </si>
   <si>
+    <t>PHYS 121</t>
+  </si>
+  <si>
     <t>MUS 104</t>
   </si>
   <si>
     <t>ENGL 114</t>
   </si>
   <si>
+    <t>COMM 100</t>
+  </si>
+  <si>
+    <t>PHYS 140</t>
+  </si>
+  <si>
     <t>MUS 106</t>
   </si>
   <si>
     <t>ENGL 115</t>
   </si>
   <si>
+    <t>COMM 115</t>
+  </si>
+  <si>
+    <t>PHYS 141</t>
+  </si>
+  <si>
     <t>MUS 110A</t>
   </si>
   <si>
     <t>ENGL 117</t>
   </si>
   <si>
+    <t>COMM 118</t>
+  </si>
+  <si>
+    <t>PHYS 142</t>
+  </si>
+  <si>
     <t>MUS 122</t>
   </si>
   <si>
     <t>ENGL 118</t>
   </si>
   <si>
+    <t>COMM 122</t>
+  </si>
+  <si>
     <t>MUS 123</t>
   </si>
   <si>
     <t>ENGL 120A</t>
   </si>
   <si>
+    <t>ECS 301</t>
+  </si>
+  <si>
     <t>MUS 125</t>
   </si>
   <si>
     <t>ENGL 120B</t>
   </si>
   <si>
+    <t>ENVS 103</t>
+  </si>
+  <si>
     <t>TD 100</t>
   </si>
   <si>
     <t>ENGL 121</t>
   </si>
   <si>
+    <t>ENVS 105</t>
+  </si>
+  <si>
     <t>TD 102</t>
   </si>
   <si>
     <t>ENGL 122</t>
   </si>
   <si>
+    <t>ENVS 107</t>
+  </si>
+  <si>
     <t>TD 109</t>
   </si>
   <si>
     <t>ENGL 123</t>
   </si>
   <si>
+    <t>ENVS 109</t>
+  </si>
+  <si>
     <t>ENGL 125A</t>
   </si>
   <si>
+    <t>GEOG 102</t>
+  </si>
+  <si>
     <t>ENGL 125B</t>
   </si>
   <si>
+    <t>GEOG 104</t>
+  </si>
+  <si>
     <t>ENGL 130</t>
   </si>
   <si>
+    <t>GEOG 105</t>
+  </si>
+  <si>
     <t>FREN 102A</t>
   </si>
   <si>
+    <t>GEOG 106</t>
+  </si>
+  <si>
     <t>FREN 102B</t>
   </si>
   <si>
+    <t>GEOG 107</t>
+  </si>
+  <si>
     <t>HIST 102A</t>
   </si>
   <si>
+    <t>GEOG 108</t>
+  </si>
+  <si>
     <t>HIST 102B</t>
   </si>
   <si>
@@ -242,6 +455,147 @@
   </si>
   <si>
     <t>HIST 106B</t>
+  </si>
+  <si>
+    <t>HIST 114A</t>
+  </si>
+  <si>
+    <t>HIST 107</t>
+  </si>
+  <si>
+    <t>HIST 114B</t>
+  </si>
+  <si>
+    <t>HIST 115</t>
+  </si>
+  <si>
+    <t>HIST 117A</t>
+  </si>
+  <si>
+    <t>HIST 117B</t>
+  </si>
+  <si>
+    <t>HIST 119A</t>
+  </si>
+  <si>
+    <t>HIST 119B</t>
+  </si>
+  <si>
+    <t>HIST 118</t>
+  </si>
+  <si>
+    <t>IS 110</t>
+  </si>
+  <si>
+    <t>IS 120</t>
+  </si>
+  <si>
+    <t>JOUR 155</t>
+  </si>
+  <si>
+    <t>JOUR 106</t>
+  </si>
+  <si>
+    <t>PS 102</t>
+  </si>
+  <si>
+    <t>JPNS 102A</t>
+  </si>
+  <si>
+    <t>PS 103</t>
+  </si>
+  <si>
+    <t>MM 100</t>
+  </si>
+  <si>
+    <t>PS 104</t>
+  </si>
+  <si>
+    <t>PHIL 100</t>
+  </si>
+  <si>
+    <t>PS 105</t>
+  </si>
+  <si>
+    <t>PHIL 101</t>
+  </si>
+  <si>
+    <t>PSY 101</t>
+  </si>
+  <si>
+    <t>PHIL 102</t>
+  </si>
+  <si>
+    <t>PSY 102</t>
+  </si>
+  <si>
+    <t>PHIL 106</t>
+  </si>
+  <si>
+    <t>PSY 106</t>
+  </si>
+  <si>
+    <t>PHIL 109A</t>
+  </si>
+  <si>
+    <t>PSY 108</t>
+  </si>
+  <si>
+    <t>PHIL 109B</t>
+  </si>
+  <si>
+    <t>PSY 112</t>
+  </si>
+  <si>
+    <t>PHIL 110</t>
+  </si>
+  <si>
+    <t>PSY 115</t>
+  </si>
+  <si>
+    <t>PHIL 112</t>
+  </si>
+  <si>
+    <t>PSY 120</t>
+  </si>
+  <si>
+    <t>PHIL 114</t>
+  </si>
+  <si>
+    <t>SOC 101</t>
+  </si>
+  <si>
+    <t>SPAN 102A</t>
+  </si>
+  <si>
+    <t>SOC 102</t>
+  </si>
+  <si>
+    <t>SPAN 102B</t>
+  </si>
+  <si>
+    <t>SOC 103</t>
+  </si>
+  <si>
+    <t>TD 107</t>
+  </si>
+  <si>
+    <t>SOC 105</t>
+  </si>
+  <si>
+    <t>WS 115</t>
+  </si>
+  <si>
+    <t>SOC 106</t>
+  </si>
+  <si>
+    <t>WS 101</t>
+  </si>
+  <si>
+    <t>WS 108</t>
+  </si>
+  <si>
+    <t>WS 120</t>
   </si>
 </sst>
 </file>
@@ -540,290 +894,745 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>53</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>60</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>67</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10">
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>73</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>78</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12">
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>83</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>40</v>
+        <v>87</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="14">
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>42</v>
+        <v>91</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>44</v>
+        <v>95</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="3" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>46</v>
+        <v>98</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" s="3" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>48</v>
+        <v>101</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="3" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
+        <v>105</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" s="3" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>52</v>
+        <v>109</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" s="3" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>54</v>
+        <v>113</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="21">
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>56</v>
+        <v>116</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" s="3" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>58</v>
+        <v>119</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23">
       <c r="C23" s="3" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>60</v>
+        <v>122</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="24">
       <c r="C24" s="3" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>62</v>
+        <v>125</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="25">
       <c r="C25" s="3" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>64</v>
+        <v>128</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="26">
       <c r="D26" s="3" t="s">
-        <v>65</v>
+        <v>130</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="27">
       <c r="D27" s="3" t="s">
-        <v>66</v>
+        <v>132</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="28">
       <c r="D28" s="3" t="s">
-        <v>67</v>
+        <v>134</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="29">
       <c r="D29" s="3" t="s">
-        <v>68</v>
+        <v>136</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" s="3" t="s">
-        <v>69</v>
+        <v>138</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" s="3" t="s">
-        <v>70</v>
+        <v>140</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" s="3" t="s">
-        <v>71</v>
+        <v>142</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" s="3" t="s">
-        <v>72</v>
+        <v>143</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" s="3" t="s">
-        <v>73</v>
+        <v>144</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" s="3" t="s">
-        <v>74</v>
+        <v>145</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" s="3" t="s">
-        <v>75</v>
+        <v>146</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" s="3" t="s">
-        <v>76</v>
+        <v>147</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="D43" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="D44" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="D45" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="D46" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="D47" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="D48" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="D49" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="D50" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="D51" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="D52" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="D53" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="D54" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="D55" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="D56" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="D57" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="D58" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="D59" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="D60" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="D61" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="D62" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="E63" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="E64" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="E65" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>